<commit_message>
TUMS client and chart
</commit_message>
<xml_diff>
--- a/src/data/data2.xlsx
+++ b/src/data/data2.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="23" windowWidth="18180" windowHeight="7403"/>
+    <workbookView xWindow="540" yWindow="20" windowWidth="17253" windowHeight="7400"/>
   </bookViews>
   <sheets>
     <sheet name="data2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -921,12 +921,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="F159" sqref="F157:F250"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.64453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>7</v>
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>8</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>9</v>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1078,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1258,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1298,7 +1298,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1318,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1338,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1358,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1378,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1418,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1438,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1498,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1518,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1538,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1558,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1578,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1598,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1638,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1658,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1678,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1698,7 +1698,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1758,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1798,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1858,7 +1858,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1898,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1958,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2058,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2098,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2118,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2138,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2158,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2178,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2198,7 +2198,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2218,7 +2218,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2238,7 +2238,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2258,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2278,7 +2278,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2298,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2397,8 +2397,8 @@
       <c r="E73" s="8">
         <v>0</v>
       </c>
-      <c r="F73" s="8">
-        <v>0</v>
+      <c r="F73" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2417,8 +2417,8 @@
       <c r="E74" s="8">
         <v>0</v>
       </c>
-      <c r="F74" s="8">
-        <v>0</v>
+      <c r="F74" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2437,8 +2437,8 @@
       <c r="E75" s="8">
         <v>0</v>
       </c>
-      <c r="F75" s="8">
-        <v>0</v>
+      <c r="F75" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2457,8 +2457,8 @@
       <c r="E76" s="8">
         <v>0</v>
       </c>
-      <c r="F76" s="8">
-        <v>0</v>
+      <c r="F76" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2478,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2498,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2518,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2558,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2578,7 +2578,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2598,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2618,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2638,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2658,7 +2658,7 @@
         <v>0</v>
       </c>
       <c r="F86" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2678,7 +2678,7 @@
         <v>0</v>
       </c>
       <c r="F87" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2698,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2718,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="F89" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2758,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2778,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="F92" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2798,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="F93" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2818,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="F94" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2838,7 +2838,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="F96" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2878,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="F97" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2898,7 +2898,7 @@
         <v>0</v>
       </c>
       <c r="F98" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2918,7 +2918,7 @@
         <v>0</v>
       </c>
       <c r="F99" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2938,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="F100" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2958,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="F101" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="F102" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2998,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="F103" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="F104" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="F105" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3058,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3078,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3098,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="F108" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3118,7 +3118,7 @@
         <v>0</v>
       </c>
       <c r="F109" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3138,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="F110" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="F111" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3178,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="F112" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3198,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="F113" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="F114" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3238,7 +3238,7 @@
         <v>0</v>
       </c>
       <c r="F115" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="F116" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="F117" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3298,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3318,7 +3318,7 @@
         <v>0</v>
       </c>
       <c r="F119" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3338,7 +3338,7 @@
         <v>0</v>
       </c>
       <c r="F120" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3358,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="F121" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -3378,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="F122" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3398,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="F123" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3418,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="F124" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3438,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="F125" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3458,7 +3458,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3478,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="F127" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3498,7 +3498,7 @@
         <v>0</v>
       </c>
       <c r="F128" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3518,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="F129" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3538,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="F130" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3558,7 +3558,7 @@
         <v>0</v>
       </c>
       <c r="F131" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3578,7 +3578,7 @@
         <v>0</v>
       </c>
       <c r="F132" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3598,7 +3598,7 @@
         <v>0</v>
       </c>
       <c r="F133" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3618,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="F134" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3638,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="F135" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3658,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="F136" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3678,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="F137" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3698,7 +3698,7 @@
         <v>0</v>
       </c>
       <c r="F138" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -3718,7 +3718,7 @@
         <v>0</v>
       </c>
       <c r="F139" s="10">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -3738,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="F140" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -3758,7 +3758,7 @@
         <v>0</v>
       </c>
       <c r="F141" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -3778,7 +3778,7 @@
         <v>0</v>
       </c>
       <c r="F142" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="F155" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -4058,7 +4058,7 @@
         <v>0</v>
       </c>
       <c r="F156" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -4078,7 +4078,7 @@
         <v>0</v>
       </c>
       <c r="F157" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -4098,7 +4098,7 @@
         <v>0</v>
       </c>
       <c r="F158" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -4118,7 +4118,7 @@
         <v>0</v>
       </c>
       <c r="F159" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -4138,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="F160" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -4158,7 +4158,7 @@
         <v>0</v>
       </c>
       <c r="F161" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -4178,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="F162" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -4198,7 +4198,7 @@
         <v>0</v>
       </c>
       <c r="F163" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -4218,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="F164" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -4238,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="F165" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -4258,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="F166" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -4278,7 +4278,7 @@
         <v>0</v>
       </c>
       <c r="F167" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="F168" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -4318,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="F169" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -4338,7 +4338,7 @@
         <v>0</v>
       </c>
       <c r="F170" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -4358,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="F171" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -4378,7 +4378,7 @@
         <v>0</v>
       </c>
       <c r="F172" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -4398,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="F173" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -4418,7 +4418,7 @@
         <v>0</v>
       </c>
       <c r="F174" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -4438,7 +4438,7 @@
         <v>0</v>
       </c>
       <c r="F175" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -4458,7 +4458,7 @@
         <v>0</v>
       </c>
       <c r="F176" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -4478,7 +4478,7 @@
         <v>0</v>
       </c>
       <c r="F177" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -4498,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="F178" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -4518,7 +4518,7 @@
         <v>0</v>
       </c>
       <c r="F179" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -4538,7 +4538,7 @@
         <v>0</v>
       </c>
       <c r="F180" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -4558,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="F181" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -4578,7 +4578,7 @@
         <v>0</v>
       </c>
       <c r="F182" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -4598,7 +4598,7 @@
         <v>0</v>
       </c>
       <c r="F183" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -4618,7 +4618,7 @@
         <v>0</v>
       </c>
       <c r="F184" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="185" spans="1:6">
@@ -4638,7 +4638,7 @@
         <v>0</v>
       </c>
       <c r="F185" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -4658,7 +4658,7 @@
         <v>0</v>
       </c>
       <c r="F186" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -4678,7 +4678,7 @@
         <v>0</v>
       </c>
       <c r="F187" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -4698,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="F188" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -4718,7 +4718,7 @@
         <v>0</v>
       </c>
       <c r="F189" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
       <c r="F190" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -4758,7 +4758,7 @@
         <v>0</v>
       </c>
       <c r="F191" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -4778,7 +4778,7 @@
         <v>0</v>
       </c>
       <c r="F192" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -4798,7 +4798,7 @@
         <v>0</v>
       </c>
       <c r="F193" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -4818,7 +4818,7 @@
         <v>0</v>
       </c>
       <c r="F194" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="195" spans="1:6">
@@ -4838,7 +4838,7 @@
         <v>0</v>
       </c>
       <c r="F195" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="196" spans="1:6">
@@ -4858,7 +4858,7 @@
         <v>0</v>
       </c>
       <c r="F196" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="197" spans="1:6">
@@ -4878,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="F197" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -4898,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="F198" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="199" spans="1:6">
@@ -4918,7 +4918,7 @@
         <v>0</v>
       </c>
       <c r="F199" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="200" spans="1:6">
@@ -4938,7 +4938,7 @@
         <v>0</v>
       </c>
       <c r="F200" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -4958,7 +4958,7 @@
         <v>0</v>
       </c>
       <c r="F201" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -4978,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="F202" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="203" spans="1:6">
@@ -4998,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="F203" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -5018,7 +5018,7 @@
         <v>0</v>
       </c>
       <c r="F204" s="10">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="205" spans="1:6">
@@ -5038,7 +5038,7 @@
         <v>0</v>
       </c>
       <c r="F205" s="10">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -5058,7 +5058,7 @@
         <v>0</v>
       </c>
       <c r="F206" s="10">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="207" spans="1:6">
@@ -5078,7 +5078,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="10">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="208" spans="1:6">
@@ -5098,7 +5098,7 @@
         <v>0</v>
       </c>
       <c r="F208" s="10">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -5118,7 +5118,7 @@
         <v>0</v>
       </c>
       <c r="F209" s="10">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="210" spans="1:6">
@@ -5138,7 +5138,7 @@
         <v>0</v>
       </c>
       <c r="F210" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="211" spans="1:6">
@@ -5158,7 +5158,7 @@
         <v>0</v>
       </c>
       <c r="F211" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -5178,7 +5178,7 @@
         <v>0</v>
       </c>
       <c r="F212" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="213" spans="1:6">
@@ -5198,7 +5198,7 @@
         <v>0</v>
       </c>
       <c r="F213" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="214" spans="1:6">
@@ -5218,7 +5218,7 @@
         <v>0</v>
       </c>
       <c r="F214" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -5238,7 +5238,7 @@
         <v>0</v>
       </c>
       <c r="F215" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -5258,7 +5258,7 @@
         <v>0</v>
       </c>
       <c r="F216" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="217" spans="1:6">
@@ -5278,7 +5278,7 @@
         <v>0</v>
       </c>
       <c r="F217" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="218" spans="1:6">
@@ -5298,7 +5298,7 @@
         <v>0</v>
       </c>
       <c r="F218" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -5318,7 +5318,7 @@
         <v>0</v>
       </c>
       <c r="F219" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -5338,7 +5338,7 @@
         <v>0</v>
       </c>
       <c r="F220" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -5358,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="F221" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -5378,7 +5378,7 @@
         <v>0</v>
       </c>
       <c r="F222" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -5398,7 +5398,7 @@
         <v>0</v>
       </c>
       <c r="F223" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="224" spans="1:6">
@@ -5418,7 +5418,7 @@
         <v>0</v>
       </c>
       <c r="F224" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -5438,7 +5438,7 @@
         <v>0</v>
       </c>
       <c r="F225" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -5458,7 +5458,7 @@
         <v>0</v>
       </c>
       <c r="F226" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -5478,7 +5478,7 @@
         <v>0</v>
       </c>
       <c r="F227" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -5498,7 +5498,7 @@
         <v>0</v>
       </c>
       <c r="F228" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -5518,7 +5518,7 @@
         <v>0</v>
       </c>
       <c r="F229" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -5538,7 +5538,7 @@
         <v>0</v>
       </c>
       <c r="F230" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -5558,7 +5558,7 @@
         <v>0</v>
       </c>
       <c r="F231" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="232" spans="1:6">
@@ -5578,7 +5578,7 @@
         <v>0</v>
       </c>
       <c r="F232" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="233" spans="1:6">
@@ -5598,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="F233" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="234" spans="1:6">
@@ -5618,7 +5618,7 @@
         <v>0</v>
       </c>
       <c r="F234" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="235" spans="1:6">
@@ -5638,7 +5638,7 @@
         <v>0</v>
       </c>
       <c r="F235" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -5658,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="F236" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -5678,7 +5678,7 @@
         <v>0</v>
       </c>
       <c r="F237" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="238" spans="1:6">
@@ -5698,7 +5698,7 @@
         <v>0</v>
       </c>
       <c r="F238" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -5718,7 +5718,7 @@
         <v>0</v>
       </c>
       <c r="F239" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -5738,7 +5738,7 @@
         <v>0</v>
       </c>
       <c r="F240" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="241" spans="1:6">
@@ -5758,7 +5758,7 @@
         <v>0</v>
       </c>
       <c r="F241" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="242" spans="1:6">
@@ -5778,7 +5778,7 @@
         <v>0</v>
       </c>
       <c r="F242" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="243" spans="1:6">
@@ -5798,7 +5798,7 @@
         <v>0</v>
       </c>
       <c r="F243" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="244" spans="1:6">
@@ -5818,7 +5818,7 @@
         <v>0</v>
       </c>
       <c r="F244" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="245" spans="1:6">
@@ -5838,7 +5838,7 @@
         <v>0</v>
       </c>
       <c r="F245" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="246" spans="1:6">
@@ -5858,7 +5858,7 @@
         <v>0</v>
       </c>
       <c r="F246" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="247" spans="1:6">
@@ -5878,7 +5878,7 @@
         <v>0</v>
       </c>
       <c r="F247" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="248" spans="1:6">
@@ -5898,7 +5898,7 @@
         <v>0</v>
       </c>
       <c r="F248" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="249" spans="1:6">
@@ -5918,7 +5918,7 @@
         <v>0</v>
       </c>
       <c r="F249" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="250" spans="1:6">
@@ -5938,10 +5938,11 @@
         <v>0</v>
       </c>
       <c r="F250" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>